<commit_message>
Vervollständigung Dokumentation Arbeitsverlauf Dimitri Khodak.xlsx
</commit_message>
<xml_diff>
--- a/Arbeitsverlauf/Dokumentation Arbeitsverlauf Dimitri Khodak.xlsx
+++ b/Arbeitsverlauf/Dokumentation Arbeitsverlauf Dimitri Khodak.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3341D4AD-A4A2-434B-9CA5-E72C73F8C4D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA66611F-C9F3-4134-9E0A-D40BD7553242}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mi, 26.02.2020" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Di, 03.03.2020" sheetId="6" r:id="rId5"/>
     <sheet name="Mi, 04.03.2020" sheetId="7" r:id="rId6"/>
     <sheet name="Do, 05.03.2020" sheetId="8" r:id="rId7"/>
+    <sheet name="Fr, 06.03.2020" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="63">
   <si>
     <t>1.</t>
   </si>
@@ -200,6 +201,21 @@
   </si>
   <si>
     <t>Erstellung von PHP-Funktionen zum Zugriff von einer mobilen App</t>
+  </si>
+  <si>
+    <t>Durch hohen Zeitdruck und eine hohe Abwesenheitsrate kann das Projektziel nicht erreicht werden</t>
+  </si>
+  <si>
+    <t>11, 12, 13</t>
+  </si>
+  <si>
+    <t>Erstellung der Doku zu Qualitätsstandards im Bezug auf das Projekt</t>
+  </si>
+  <si>
+    <t>Reflektive Einsichten und schriftliche Doku der Qualitätskriterien im Bezug auf die ISO 25010</t>
+  </si>
+  <si>
+    <t>Optimierung des Kostenanalyseplans</t>
   </si>
 </sst>
 </file>
@@ -1528,8 +1544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0ABA197-0C93-425E-B1F6-3337A64111B6}">
   <dimension ref="B1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1694,7 +1710,12 @@
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D23" s="16"/>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="16">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D24" s="16"/>
@@ -1705,4 +1726,182 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E13D8F-B92F-41EE-B491-E46B3BA9E790}">
+  <dimension ref="B1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="101.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="71.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="10">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="3"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="3"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="16"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="16"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>